<commit_message>
update SSCS Pin List
</commit_message>
<xml_diff>
--- a/SSCS Chipathon Pin List.xlsx
+++ b/SSCS Chipathon Pin List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christof Gindu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\_Masterarbeit\pll2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE279F90-05E7-4A90-9D43-73DD995FA06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843A83D8-3DE0-40A3-B3E1-CB8B05272F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Team name:</t>
   </si>
@@ -103,9 +103,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>(add more lines if needed)</t>
-  </si>
-  <si>
     <t>Austria 1</t>
   </si>
   <si>
@@ -151,7 +148,37 @@
     <t>vddc1</t>
   </si>
   <si>
-    <t>0.006</t>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>estimate</t>
+  </si>
+  <si>
+    <t>clock</t>
+  </si>
+  <si>
+    <t>clk</t>
+  </si>
+  <si>
+    <t>dig_in</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>dig_out</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>sensitive</t>
+  </si>
+  <si>
+    <t>special considerations:</t>
+  </si>
+  <si>
+    <t>The VCO supply is quite sensitive, please consider this when layouting the complete Caravan!</t>
   </si>
 </sst>
 </file>
@@ -199,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -218,6 +245,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,7 +470,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -461,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -469,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -477,6 +507,9 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -485,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -493,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -619,13 +652,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>18</v>
@@ -640,13 +673,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>18</v>
@@ -661,13 +694,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>18</v>
@@ -676,19 +709,22 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
+      <c r="J13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>18</v>
@@ -697,19 +733,22 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="7" t="s">
@@ -724,13 +763,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -740,49 +779,119 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>11</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
       <c r="B22" s="8"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>